<commit_message>
calibration steps up to 11-26
</commit_message>
<xml_diff>
--- a/data/incidence_crude.xlsx
+++ b/data/incidence_crude.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/st3381_cumc_columbia_edu/Documents/HIRE/CRC Screening Models/NH Calibration US/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/st3381_cumc_columbia_edu/Documents/HIRE/CRC Screening Models/dr-crc-calibration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="8_{FDA6DDAD-F19B-4FDF-A9C9-DB3DB4C3EAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF0CA6D0-4ACD-4824-AA46-719F734EB88E}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="8_{FDA6DDAD-F19B-4FDF-A9C9-DB3DB4C3EAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49DE66DE-3080-43EE-8E99-5ACA03FB7DA5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2355" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{DCC8D167-734C-4950-A727-251B7B1C9C55}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{DCC8D167-734C-4950-A727-251B7B1C9C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -517,6 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,12 +858,12 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -986,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>7.84</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>6.387096774193548</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>12.692307692307692</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>11.09090909090909</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>18.046153846153846</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>21.666666666666668</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>29.16</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1958,7 +1959,7 @@
         <v>36.518518518518519</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>29.495798319327733</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>49.030864197530867</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>44.11392405063291</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2282,7 +2283,7 @@
         <v>39.361702127659576</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>56.33653846153846</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>63.14453125</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>83.128919860627178</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2606,7 +2607,7 @@
         <v>87.527027027027032</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>77.418478260869563</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2768,7 +2769,7 @@
         <v>119.53990610328638</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>119.72279260780287</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>143.01923076923077</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>118.20738137082601</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -3092,7 +3093,7 @@
         <v>159.193893129771</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>146.82478632478632</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>176.69152970922883</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -3335,7 +3336,7 @@
         <v>187.57211538461539</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -3416,7 +3417,7 @@
         <v>226.85345717234262</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>222.55048287971906</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3578,7 +3579,7 @@
         <v>239.0174978127734</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -3659,7 +3660,7 @@
         <v>260.52173913043481</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3740,7 +3741,7 @@
         <v>269.05779889152814</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>287.61890694239293</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>292.64199288256225</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3983,7 +3984,7 @@
         <v>320.5042455911169</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -4064,7 +4065,7 @@
         <v>325.57875000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>356.03801169590645</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>341.72653282691266</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4307,7 +4308,7 @@
         <v>408.78560250391234</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>426.2872238232469</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>418.51455399061035</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -4550,7 +4551,7 @@
         <v>460.13994685562443</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>474.96447973255329</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>507.54531250000002</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -4793,7 +4794,7 @@
         <v>516.3120567375887</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -4874,7 +4875,7 @@
         <v>541.28718300205617</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -4955,7 +4956,7 @@
         <v>556.55106888361047</v>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -5036,7 +5037,7 @@
         <v>665.80089058524175</v>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>653.90723562152129</v>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -5198,7 +5199,7 @@
         <v>607.0873726458783</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>613.88888888888891</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>665.11771332019146</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -5441,7 +5442,7 @@
         <v>612.58168389955688</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -5522,7 +5523,7 @@
         <v>623.45114345114348</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -5603,7 +5604,7 @@
         <v>609.18061674008811</v>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -5684,7 +5685,7 @@
         <v>618.55683192261188</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>589.7094936708861</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>534.49950347567028</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -5927,7 +5928,7 @@
         <v>550.87944463257702</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -6008,7 +6009,7 @@
         <v>559.38336347197105</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -6089,7 +6090,7 @@
         <v>481.66864608076008</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -6170,7 +6171,7 @@
         <v>496.40151515151513</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>434.83641536273115</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -6332,7 +6333,7 @@
         <v>2414.9413894977606</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>80</v>
       </c>
@@ -6410,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -6447,12 +6448,12 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6481,7 +6482,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -6531,7 +6532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -6595,7 +6596,7 @@
         <v>9.7358114543282137E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6659,7 +6660,7 @@
         <v>7.3077780335500095E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -6723,7 +6724,7 @@
         <v>0.1505247171219096</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>0.16687889211640081</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6851,7 +6852,7 @@
         <v>0.17547224751971993</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -6915,7 +6916,7 @@
         <v>0.13761110089568773</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -6979,7 +6980,7 @@
         <v>0.27190278259375278</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -7043,7 +7044,7 @@
         <v>0.22874565240294398</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -7107,7 +7108,7 @@
         <v>0.37011169185201004</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>0.41702265966402219</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -7235,7 +7236,7 @@
         <v>0.5440626366103779</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -7299,7 +7300,7 @@
         <v>0.70869025968416433</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -7363,7 +7364,7 @@
         <v>0.56635938066649316</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -7427,7 +7428,7 @@
         <v>0.95073861174696783</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -7491,7 +7492,7 @@
         <v>0.8324101224338426</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -7555,7 +7556,7 @@
         <v>0.72892013980105153</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>1.0821103805336176</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -7683,7 +7684,7 @@
         <v>1.224494399028542</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -7747,7 +7748,7 @@
         <v>1.6778112455105338</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -7811,7 +7812,7 @@
         <v>1.7219557310145528</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -7875,7 +7876,7 @@
         <v>1.5341358527753415</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -7939,7 +7940,7 @@
         <v>2.5370396858619966</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -8003,7 +8004,7 @@
         <v>2.575861961112166</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -8067,7 +8068,7 @@
         <v>3.1850998075886214</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -8131,7 +8132,7 @@
         <v>2.6645915116380605</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -8195,7 +8196,7 @@
         <v>3.6046615389545043</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -8259,7 +8260,7 @@
         <v>3.5940616523475883</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -8323,7 +8324,7 @@
         <v>4.4568179898920679</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>5.0582626811001949</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -8451,7 +8452,7 @@
         <v>6.0461718779692051</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -8515,7 +8516,7 @@
         <v>6.1230574468300505</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -8579,7 +8580,7 @@
         <v>7.20639186734617</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -8643,7 +8644,7 @@
         <v>8.2417506842908814</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -8707,7 +8708,7 @@
         <v>9.0539966285828157</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -8771,7 +8772,7 @@
         <v>10.070020094685329</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -8835,7 +8836,7 @@
         <v>10.832967210454505</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -8899,7 +8900,7 @@
         <v>12.499561081722916</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>13.250491329844406</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -9027,7 +9028,7 @@
         <v>15.63356430026001</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>15.227016557567319</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>18.605274494534161</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -9219,7 +9220,7 @@
         <v>20.560063848712698</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -9283,7 +9284,7 @@
         <v>20.462127507653371</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -9347,7 +9348,7 @@
         <v>22.816547619798762</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -9411,7 +9412,7 @@
         <v>23.703708422210752</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -9475,7 +9476,7 @@
         <v>25.638224290945388</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>26.744326312403977</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -9603,7 +9604,7 @@
         <v>28.280446635892837</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -9667,7 +9668,7 @@
         <v>30.274818388625029</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -9731,7 +9732,7 @@
         <v>36.170932722331237</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>36.103535535640532</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -9859,7 +9860,7 @@
         <v>35.048684255410883</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -9923,7 +9924,7 @@
         <v>36.507865710524015</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -9987,7 +9988,7 @@
         <v>40.924830596276408</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -10051,7 +10052,7 @@
         <v>38.884989659530781</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -10115,7 +10116,7 @@
         <v>41.013473567500803</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -10179,7 +10180,7 @@
         <v>42.871452400412409</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -10243,7 +10244,7 @@
         <v>46.298990791397628</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -10307,7 +10308,7 @@
         <v>46.680933292610099</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -10371,7 +10372,7 @@
         <v>45.648253064556705</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -10435,7 +10436,7 @@
         <v>50.920884778309514</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -10499,7 +10500,7 @@
         <v>58.003372411802083</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -10563,7 +10564,7 @@
         <v>54.260479204138356</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -10627,7 +10628,7 @@
         <v>61.9101177525243</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -10691,7 +10692,7 @@
         <v>60.40585995609289</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -10755,7 +10756,7 @@
         <v>63.981313015777687</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -10783,7 +10784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F70">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -10793,7 +10794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -10813,20 +10814,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC672811-E14E-449E-94DD-B3046D62311B}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -10840,7 +10841,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -10854,7 +10855,7 @@
         <v>4.7343259260373381E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>21</v>
       </c>
@@ -10868,7 +10869,7 @@
         <v>3.9964663244758988E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22</v>
       </c>
@@ -10882,7 +10883,7 @@
         <v>6.3073111976886448E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>23</v>
       </c>
@@ -10896,7 +10897,7 @@
         <v>0.18756397791117241</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -10910,7 +10911,7 @@
         <v>0.11758577759082769</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -10924,7 +10925,7 @@
         <v>0.24102087018887081</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>26</v>
       </c>
@@ -10938,7 +10939,7 @@
         <v>0.23753049721919653</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27</v>
       </c>
@@ -10952,7 +10953,7 @@
         <v>0.26824997818457053</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>28</v>
       </c>
@@ -10966,7 +10967,7 @@
         <v>0.23640668138755408</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>29</v>
       </c>
@@ -10980,7 +10981,7 @@
         <v>0.43743056022862714</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>30</v>
       </c>
@@ -10994,7 +10995,7 @@
         <v>0.44409594472390573</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>31</v>
       </c>
@@ -11008,7 +11009,7 @@
         <v>0.49448034556159182</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>32</v>
       </c>
@@ -11022,7 +11023,7 @@
         <v>0.71136652540644263</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>33</v>
       </c>
@@ -11036,7 +11037,7 @@
         <v>0.82976551767639684</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -11050,7 +11051,7 @@
         <v>0.65668474022268064</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>35</v>
       </c>
@@ -11064,7 +11065,7 @@
         <v>1.2609376868144508</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>36</v>
       </c>
@@ -11078,7 +11079,7 @@
         <v>1.2347660888904508</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>37</v>
       </c>
@@ -11092,7 +11093,7 @@
         <v>1.1961039826810598</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>38</v>
       </c>
@@ -11106,7 +11107,7 @@
         <v>1.5326926221192447</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>39</v>
       </c>
@@ -11120,7 +11121,7 @@
         <v>1.7983217028036231</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>40</v>
       </c>
@@ -11134,7 +11135,7 @@
         <v>1.9947183765678538</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>41</v>
       </c>
@@ -11148,7 +11149,7 @@
         <v>2.0517946050621103</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>42</v>
       </c>
@@ -11162,7 +11163,7 @@
         <v>2.2422535430753481</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>43</v>
       </c>
@@ -11176,7 +11177,7 @@
         <v>2.4882718156523791</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>44</v>
       </c>
@@ -11190,7 +11191,7 @@
         <v>3.0464202186943701</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>45</v>
       </c>
@@ -11204,7 +11205,7 @@
         <v>4.1174055257170137</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>46</v>
       </c>
@@ -11218,7 +11219,7 @@
         <v>4.0214361802599736</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>47</v>
       </c>
@@ -11232,7 +11233,7 @@
         <v>5.1074642676397719</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>48</v>
       </c>
@@ -11246,7 +11247,7 @@
         <v>6.7589466724185296</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>49</v>
       </c>
@@ -11260,7 +11261,7 @@
         <v>6.4364144650980091</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>50</v>
       </c>
@@ -11274,7 +11275,7 @@
         <v>7.9690893897617308</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>51</v>
       </c>
@@ -11288,7 +11289,7 @@
         <v>8.3729787144945025</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>52</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>10.15978057385883</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>53</v>
       </c>
@@ -11316,7 +11317,7 @@
         <v>11.291439627933919</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>54</v>
       </c>
@@ -11330,7 +11331,7 @@
         <v>12.328695704093212</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>55</v>
       </c>
@@ -11344,7 +11345,7 @@
         <v>12.975451348712919</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>56</v>
       </c>
@@ -11358,7 +11359,7 @@
         <v>14.211506086220567</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>57</v>
       </c>
@@ -11372,7 +11373,7 @@
         <v>17.007946417209588</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>58</v>
       </c>
@@ -11386,7 +11387,7 @@
         <v>18.582812472981008</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>59</v>
       </c>
@@ -11400,7 +11401,7 @@
         <v>19.54650373759781</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>60</v>
       </c>
@@ -11414,7 +11415,7 @@
         <v>21.864848282925063</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>61</v>
       </c>
@@ -11428,7 +11429,7 @@
         <v>23.110733688992052</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>62</v>
       </c>
@@ -11442,7 +11443,7 @@
         <v>26.414844359359019</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>63</v>
       </c>
@@ -11456,7 +11457,7 @@
         <v>26.386232406946057</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>64</v>
       </c>
@@ -11470,7 +11471,7 @@
         <v>27.802129722730715</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>65</v>
       </c>
@@ -11484,7 +11485,7 @@
         <v>32.542089833392012</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>66</v>
       </c>
@@ -11498,7 +11499,7 @@
         <v>32.963595523163264</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>67</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>37.554516337203673</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>68</v>
       </c>
@@ -11526,7 +11527,7 @@
         <v>37.355432435470874</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>69</v>
       </c>
@@ -11540,7 +11541,7 @@
         <v>39.759628155286791</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>70</v>
       </c>
@@ -11554,7 +11555,7 @@
         <v>43.726832472971189</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>71</v>
       </c>
@@ -11568,7 +11569,7 @@
         <v>46.832055217651167</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>72</v>
       </c>
@@ -11582,7 +11583,7 @@
         <v>49.602473808231366</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>73</v>
       </c>
@@ -11596,7 +11597,7 @@
         <v>51.900331945218518</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>74</v>
       </c>
@@ -11610,7 +11611,7 @@
         <v>51.380103368451223</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>75</v>
       </c>
@@ -11624,7 +11625,7 @@
         <v>55.17578360282829</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>76</v>
       </c>
@@ -11638,7 +11639,7 @@
         <v>60.322692066407242</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>77</v>
       </c>
@@ -11652,7 +11653,7 @@
         <v>60.886864205741766</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>78</v>
       </c>
@@ -11666,7 +11667,7 @@
         <v>65.292577069207852</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>79</v>
       </c>
@@ -11680,7 +11681,7 @@
         <v>61.905717074147532</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>80</v>
       </c>
@@ -11694,7 +11695,7 @@
         <v>73.883529967452077</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>81</v>
       </c>
@@ -11708,7 +11709,7 @@
         <v>71.188246673020444</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>82</v>
       </c>
@@ -11722,7 +11723,7 @@
         <v>73.861061983271028</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>83</v>
       </c>
@@ -11736,7 +11737,7 @@
         <v>69.173931927951557</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>84</v>
       </c>
@@ -11750,7 +11751,7 @@
         <v>75.45643850291053</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>85</v>
       </c>
@@ -11763,6 +11764,9 @@
       <c r="D67">
         <v>84.936317931401362</v>
       </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11777,18 +11781,18 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" customWidth="1"/>
     <col min="26" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -11817,7 +11821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -11882,7 +11886,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11961,7 +11965,7 @@
         <v>4.7343259260373381E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -12040,7 +12044,7 @@
         <v>3.9964663244758988E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -12119,7 +12123,7 @@
         <v>6.3073111976886448E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -12198,7 +12202,7 @@
         <v>0.18756397791117241</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -12277,7 +12281,7 @@
         <v>0.11758577759082769</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -12356,7 +12360,7 @@
         <v>0.24102087018887081</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -12435,7 +12439,7 @@
         <v>0.23753049721919653</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -12514,7 +12518,7 @@
         <v>0.26824997818457053</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -12593,7 +12597,7 @@
         <v>0.23640668138755408</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -12672,7 +12676,7 @@
         <v>0.43743056022862714</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -12751,7 +12755,7 @@
         <v>0.44409594472390573</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -12830,7 +12834,7 @@
         <v>0.49448034556159182</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -12909,7 +12913,7 @@
         <v>0.71136652540644263</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -12988,7 +12992,7 @@
         <v>0.82976551767639684</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -13067,7 +13071,7 @@
         <v>0.65668474022268064</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -13146,7 +13150,7 @@
         <v>1.2609376868144508</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -13225,7 +13229,7 @@
         <v>1.2347660888904508</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -13304,7 +13308,7 @@
         <v>1.1961039826810598</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -13383,7 +13387,7 @@
         <v>1.5326926221192447</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -13462,7 +13466,7 @@
         <v>1.7983217028036231</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -13541,7 +13545,7 @@
         <v>1.9947183765678538</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -13620,7 +13624,7 @@
         <v>2.0517946050621103</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -13699,7 +13703,7 @@
         <v>2.2422535430753481</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -13778,7 +13782,7 @@
         <v>2.4882718156523791</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -13857,7 +13861,7 @@
         <v>3.0464202186943701</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -13936,7 +13940,7 @@
         <v>4.1174055257170137</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -14015,7 +14019,7 @@
         <v>4.0214361802599736</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -14094,7 +14098,7 @@
         <v>5.1074642676397719</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -14173,7 +14177,7 @@
         <v>6.7589466724185296</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -14252,7 +14256,7 @@
         <v>6.4364144650980091</v>
       </c>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -14331,7 +14335,7 @@
         <v>7.9690893897617308</v>
       </c>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -14410,7 +14414,7 @@
         <v>8.3729787144945025</v>
       </c>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -14489,7 +14493,7 @@
         <v>10.15978057385883</v>
       </c>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -14568,7 +14572,7 @@
         <v>11.291439627933919</v>
       </c>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -14647,7 +14651,7 @@
         <v>12.328695704093212</v>
       </c>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -14726,7 +14730,7 @@
         <v>12.975451348712919</v>
       </c>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -14805,7 +14809,7 @@
         <v>14.211506086220567</v>
       </c>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -14884,7 +14888,7 @@
         <v>17.007946417209588</v>
       </c>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -14963,7 +14967,7 @@
         <v>18.582812472981008</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -15042,7 +15046,7 @@
         <v>19.54650373759781</v>
       </c>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -15121,7 +15125,7 @@
         <v>21.864848282925063</v>
       </c>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -15200,7 +15204,7 @@
         <v>23.110733688992052</v>
       </c>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -15279,7 +15283,7 @@
         <v>26.414844359359019</v>
       </c>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -15358,7 +15362,7 @@
         <v>26.386232406946057</v>
       </c>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -15437,7 +15441,7 @@
         <v>27.802129722730715</v>
       </c>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -15516,7 +15520,7 @@
         <v>32.542089833392012</v>
       </c>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -15595,7 +15599,7 @@
         <v>32.963595523163264</v>
       </c>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -15674,7 +15678,7 @@
         <v>37.554516337203673</v>
       </c>
     </row>
-    <row r="51" spans="1:26">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -15753,7 +15757,7 @@
         <v>37.355432435470874</v>
       </c>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -15832,7 +15836,7 @@
         <v>39.759628155286791</v>
       </c>
     </row>
-    <row r="53" spans="1:26">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -15911,7 +15915,7 @@
         <v>43.726832472971189</v>
       </c>
     </row>
-    <row r="54" spans="1:26">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -15990,7 +15994,7 @@
         <v>46.832055217651167</v>
       </c>
     </row>
-    <row r="55" spans="1:26">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -16069,7 +16073,7 @@
         <v>49.602473808231366</v>
       </c>
     </row>
-    <row r="56" spans="1:26">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -16148,7 +16152,7 @@
         <v>51.900331945218518</v>
       </c>
     </row>
-    <row r="57" spans="1:26">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -16227,7 +16231,7 @@
         <v>51.380103368451223</v>
       </c>
     </row>
-    <row r="58" spans="1:26">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -16306,7 +16310,7 @@
         <v>55.17578360282829</v>
       </c>
     </row>
-    <row r="59" spans="1:26">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -16385,7 +16389,7 @@
         <v>60.322692066407242</v>
       </c>
     </row>
-    <row r="60" spans="1:26">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -16464,7 +16468,7 @@
         <v>60.886864205741766</v>
       </c>
     </row>
-    <row r="61" spans="1:26">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -16543,7 +16547,7 @@
         <v>65.292577069207852</v>
       </c>
     </row>
-    <row r="62" spans="1:26">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -16622,7 +16626,7 @@
         <v>61.905717074147532</v>
       </c>
     </row>
-    <row r="63" spans="1:26">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -16701,7 +16705,7 @@
         <v>73.883529967452077</v>
       </c>
     </row>
-    <row r="64" spans="1:26">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -16780,7 +16784,7 @@
         <v>71.188246673020444</v>
       </c>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -16859,7 +16863,7 @@
         <v>73.861061983271028</v>
       </c>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -16938,7 +16942,7 @@
         <v>69.173931927951557</v>
       </c>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -16974,7 +16978,7 @@
         <v>2316</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67:M98" si="14">L67-J67</f>
+        <f t="shared" ref="M67:M68" si="14">L67-J67</f>
         <v>1981</v>
       </c>
       <c r="N67" s="1">
@@ -17017,7 +17021,7 @@
         <v>75.45643850291053</v>
       </c>
     </row>
-    <row r="68" spans="1:26">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -17096,7 +17100,7 @@
         <v>84.936317931401362</v>
       </c>
     </row>
-    <row r="69" spans="1:26">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -17131,12 +17135,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:26">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:26">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -17163,9 +17167,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -17179,7 +17183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -17193,7 +17197,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>21</v>
       </c>
@@ -17207,7 +17211,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22</v>
       </c>
@@ -17221,7 +17225,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>23</v>
       </c>
@@ -17235,7 +17239,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -17249,7 +17253,7 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -17263,7 +17267,7 @@
         <v>0.29268292682926828</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>26</v>
       </c>
@@ -17277,7 +17281,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27</v>
       </c>
@@ -17291,7 +17295,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>28</v>
       </c>
@@ -17305,7 +17309,7 @@
         <v>0.20370370370370369</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>29</v>
       </c>
@@ -17319,7 +17323,7 @@
         <v>0.29333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>30</v>
       </c>
@@ -17333,7 +17337,7 @@
         <v>0.2558139534883721</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>31</v>
       </c>
@@ -17347,7 +17351,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>32</v>
       </c>
@@ -17361,7 +17365,7 @@
         <v>0.29807692307692307</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>33</v>
       </c>
@@ -17375,7 +17379,7 @@
         <v>0.2975206611570248</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -17389,7 +17393,7 @@
         <v>0.21739130434782608</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>35</v>
       </c>
@@ -17403,7 +17407,7 @@
         <v>0.32121212121212123</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>36</v>
       </c>
@@ -17417,7 +17421,7 @@
         <v>0.26595744680851063</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>37</v>
       </c>
@@ -17431,7 +17435,7 @@
         <v>0.24338624338624337</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>38</v>
       </c>
@@ -17445,7 +17449,7 @@
         <v>0.26415094339622641</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>39</v>
       </c>
@@ -17459,7 +17463,7 @@
         <v>0.24814814814814815</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>40</v>
       </c>
@@ -17473,7 +17477,7 @@
         <v>0.22812499999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>41</v>
       </c>
@@ -17487,7 +17491,7 @@
         <v>0.20474777448071216</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>42</v>
       </c>
@@ -17501,7 +17505,7 @@
         <v>0.21661721068249259</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>43</v>
       </c>
@@ -17515,7 +17519,7 @@
         <v>0.20519480519480521</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>44</v>
       </c>
@@ -17529,7 +17533,7 @@
         <v>0.23308270676691728</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>45</v>
       </c>
@@ -17543,7 +17547,7 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>46</v>
       </c>
@@ -17557,7 +17561,7 @@
         <v>0.20176991150442478</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>47</v>
       </c>
@@ -17571,7 +17575,7 @@
         <v>0.21083455344070279</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>48</v>
       </c>
@@ -17585,7 +17589,7 @@
         <v>0.23591087811271297</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>49</v>
       </c>
@@ -17599,7 +17603,7 @@
         <v>0.2126642771804062</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>50</v>
       </c>
@@ -17613,7 +17617,7 @@
         <v>0.22383419689119172</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>51</v>
       </c>
@@ -17627,7 +17631,7 @@
         <v>0.20366972477064221</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>52</v>
       </c>
@@ -17641,7 +17645,7 @@
         <v>0.2099056603773585</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>53</v>
       </c>
@@ -17655,7 +17659,7 @@
         <v>0.2092372288313506</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>54</v>
       </c>
@@ -17669,7 +17673,7 @@
         <v>0.21363040629095675</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>55</v>
       </c>
@@ -17683,7 +17687,7 @@
         <v>0.21118793211816467</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>56</v>
       </c>
@@ -17697,7 +17701,7 @@
         <v>0.20076586433260393</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>57</v>
       </c>
@@ -17711,7 +17715,7 @@
         <v>0.2081145584725537</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>58</v>
       </c>
@@ -17725,7 +17729,7 @@
         <v>0.20151245551601424</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>59</v>
       </c>
@@ -17739,7 +17743,7 @@
         <v>0.2011423908608731</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>60</v>
       </c>
@@ -17753,7 +17757,7 @@
         <v>0.200529701097238</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>61</v>
       </c>
@@ -17767,7 +17771,7 @@
         <v>0.19489723600283487</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>62</v>
       </c>
@@ -17781,7 +17785,7 @@
         <v>0.20676691729323307</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>63</v>
       </c>
@@ -17795,7 +17799,7 @@
         <v>0.19089147286821706</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>64</v>
       </c>
@@ -17809,7 +17813,7 @@
         <v>0.19094854308741477</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>65</v>
       </c>
@@ -17823,7 +17827,7 @@
         <v>0.20463887257780389</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>66</v>
       </c>
@@ -17837,7 +17841,7 @@
         <v>0.19363166953528399</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>67</v>
       </c>
@@ -17851,7 +17855,7 @@
         <v>0.20359771054783321</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>68</v>
       </c>
@@ -17865,7 +17869,7 @@
         <v>0.19158751696065129</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>69</v>
       </c>
@@ -17879,7 +17883,7 @@
         <v>0.19514148424986652</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>70</v>
       </c>
@@ -17893,7 +17897,7 @@
         <v>0.19630118890356671</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>71</v>
       </c>
@@ -17907,7 +17911,7 @@
         <v>0.20126448893572182</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>72</v>
       </c>
@@ -17921,7 +17925,7 @@
         <v>0.20309530274232962</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>73</v>
       </c>
@@ -17935,7 +17939,7 @@
         <v>0.19782262347318108</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>74</v>
       </c>
@@ -17949,7 +17953,7 @@
         <v>0.18519508284339925</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>75</v>
       </c>
@@ -17963,7 +17967,7 @@
         <v>0.18901278215936906</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>76</v>
       </c>
@@ -17977,7 +17981,7 @@
         <v>0.19943422913719944</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>77</v>
       </c>
@@ -17991,7 +17995,7 @@
         <v>0.19576877234803336</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>78</v>
       </c>
@@ -18005,7 +18009,7 @@
         <v>0.2001218397806884</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>79</v>
       </c>
@@ -18019,7 +18023,7 @@
         <v>0.18556027442012415</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>80</v>
       </c>
@@ -18033,7 +18037,7 @@
         <v>0.20795214637579171</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>81</v>
       </c>
@@ -18047,7 +18051,7 @@
         <v>0.18890074706510138</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>82</v>
       </c>
@@ -18061,7 +18065,7 @@
         <v>0.20212331563903635</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>83</v>
       </c>
@@ -18075,7 +18079,7 @@
         <v>0.18229854689564068</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>84</v>
       </c>
@@ -18089,7 +18093,7 @@
         <v>0.20090863200403836</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -18116,9 +18120,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -18132,7 +18136,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -18146,7 +18150,7 @@
         <v>0.24382700632700638</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>25</v>
       </c>
@@ -18160,7 +18164,7 @@
         <v>0.2750868499161182</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -18174,7 +18178,7 @@
         <v>0.25976056841402917</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>35</v>
       </c>
@@ -18188,7 +18192,7 @@
         <v>0.26857098059024997</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -18202,7 +18206,7 @@
         <v>0.21755349942498547</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>45</v>
       </c>
@@ -18216,7 +18220,7 @@
         <v>0.22063592404764931</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>50</v>
       </c>
@@ -18230,7 +18234,7 @@
         <v>0.21205544343229987</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>55</v>
       </c>
@@ -18244,7 +18248,7 @@
         <v>0.20454464026004193</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>60</v>
       </c>
@@ -18258,7 +18262,7 @@
         <v>0.19680677406978753</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>65</v>
       </c>
@@ -18272,7 +18276,7 @@
         <v>0.19771945077428776</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>70</v>
       </c>
@@ -18286,7 +18290,7 @@
         <v>0.19673573737963967</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>75</v>
       </c>
@@ -18300,7 +18304,7 @@
         <v>0.19397957956908285</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>80</v>
       </c>
@@ -18327,17 +18331,17 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -18345,7 +18349,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -18371,7 +18375,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
@@ -18397,7 +18401,7 @@
         <v>4.7343259260373381E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>21</v>
       </c>
@@ -18423,7 +18427,7 @@
         <v>3.9964663244758988E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>22</v>
       </c>
@@ -18449,7 +18453,7 @@
         <v>6.3073111976886448E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>23</v>
       </c>
@@ -18475,7 +18479,7 @@
         <v>0.18756397791117241</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
@@ -18501,7 +18505,7 @@
         <v>0.11758577759082769</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>25</v>
       </c>
@@ -18527,7 +18531,7 @@
         <v>0.24102087018887081</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>26</v>
       </c>
@@ -18553,7 +18557,7 @@
         <v>0.23753049721919653</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>27</v>
       </c>
@@ -18579,7 +18583,7 @@
         <v>0.26824997818457053</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>28</v>
       </c>
@@ -18605,7 +18609,7 @@
         <v>0.23640668138755408</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>29</v>
       </c>
@@ -18631,7 +18635,7 @@
         <v>0.43743056022862714</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>30</v>
       </c>
@@ -18657,7 +18661,7 @@
         <v>0.44409594472390573</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>31</v>
       </c>
@@ -18683,7 +18687,7 @@
         <v>0.49448034556159182</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>32</v>
       </c>
@@ -18709,7 +18713,7 @@
         <v>0.71136652540644263</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>33</v>
       </c>
@@ -18735,7 +18739,7 @@
         <v>0.82976551767639684</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>34</v>
       </c>
@@ -18761,7 +18765,7 @@
         <v>0.65668474022268064</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>35</v>
       </c>
@@ -18787,7 +18791,7 @@
         <v>1.2609376868144508</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>36</v>
       </c>
@@ -18813,7 +18817,7 @@
         <v>1.2347660888904508</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>37</v>
       </c>
@@ -18839,7 +18843,7 @@
         <v>1.1961039826810598</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>38</v>
       </c>
@@ -18865,7 +18869,7 @@
         <v>1.5326926221192447</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>39</v>
       </c>
@@ -18891,7 +18895,7 @@
         <v>1.7983217028036231</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>40</v>
       </c>
@@ -18917,7 +18921,7 @@
         <v>1.9947183765678538</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>41</v>
       </c>
@@ -18943,7 +18947,7 @@
         <v>2.0517946050621103</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>42</v>
       </c>
@@ -18969,7 +18973,7 @@
         <v>2.2422535430753481</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>43</v>
       </c>
@@ -18995,7 +18999,7 @@
         <v>2.4882718156523791</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>44</v>
       </c>
@@ -19021,7 +19025,7 @@
         <v>3.0464202186943701</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>45</v>
       </c>
@@ -19047,7 +19051,7 @@
         <v>4.1174055257170137</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>46</v>
       </c>
@@ -19073,7 +19077,7 @@
         <v>4.0214361802599736</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>47</v>
       </c>
@@ -19099,7 +19103,7 @@
         <v>5.1074642676397719</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>48</v>
       </c>
@@ -19125,7 +19129,7 @@
         <v>6.7589466724185296</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>49</v>
       </c>
@@ -19151,7 +19155,7 @@
         <v>6.4364144650980091</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>50</v>
       </c>
@@ -19177,7 +19181,7 @@
         <v>7.9690893897617308</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>51</v>
       </c>
@@ -19203,7 +19207,7 @@
         <v>8.3729787144945025</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>52</v>
       </c>
@@ -19229,7 +19233,7 @@
         <v>10.15978057385883</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>53</v>
       </c>
@@ -19255,7 +19259,7 @@
         <v>11.291439627933919</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>54</v>
       </c>
@@ -19281,7 +19285,7 @@
         <v>12.328695704093212</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>55</v>
       </c>
@@ -19307,7 +19311,7 @@
         <v>12.975451348712919</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>56</v>
       </c>
@@ -19333,7 +19337,7 @@
         <v>14.211506086220567</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>57</v>
       </c>
@@ -19359,7 +19363,7 @@
         <v>17.007946417209588</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>58</v>
       </c>
@@ -19385,7 +19389,7 @@
         <v>18.582812472981008</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>59</v>
       </c>
@@ -19411,7 +19415,7 @@
         <v>19.54650373759781</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>60</v>
       </c>
@@ -19437,7 +19441,7 @@
         <v>21.864848282925063</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>61</v>
       </c>
@@ -19463,7 +19467,7 @@
         <v>23.110733688992052</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>62</v>
       </c>
@@ -19489,7 +19493,7 @@
         <v>26.414844359359019</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>63</v>
       </c>
@@ -19515,7 +19519,7 @@
         <v>26.386232406946057</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>64</v>
       </c>
@@ -19541,7 +19545,7 @@
         <v>27.802129722730715</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>65</v>
       </c>
@@ -19567,7 +19571,7 @@
         <v>32.542089833392012</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>66</v>
       </c>
@@ -19593,7 +19597,7 @@
         <v>32.963595523163264</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>67</v>
       </c>
@@ -19619,7 +19623,7 @@
         <v>37.554516337203673</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>68</v>
       </c>
@@ -19645,7 +19649,7 @@
         <v>37.355432435470874</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>69</v>
       </c>
@@ -19671,7 +19675,7 @@
         <v>39.759628155286791</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>70</v>
       </c>
@@ -19697,7 +19701,7 @@
         <v>43.726832472971189</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>71</v>
       </c>
@@ -19723,7 +19727,7 @@
         <v>46.832055217651167</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>72</v>
       </c>
@@ -19749,7 +19753,7 @@
         <v>49.602473808231366</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>73</v>
       </c>
@@ -19775,7 +19779,7 @@
         <v>51.900331945218518</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>74</v>
       </c>
@@ -19801,7 +19805,7 @@
         <v>51.380103368451223</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>75</v>
       </c>
@@ -19827,7 +19831,7 @@
         <v>55.17578360282829</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>76</v>
       </c>
@@ -19853,7 +19857,7 @@
         <v>60.322692066407242</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>77</v>
       </c>
@@ -19879,7 +19883,7 @@
         <v>60.886864205741766</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>78</v>
       </c>
@@ -19905,7 +19909,7 @@
         <v>65.292577069207852</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>79</v>
       </c>
@@ -19931,7 +19935,7 @@
         <v>61.905717074147532</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>80</v>
       </c>
@@ -19957,7 +19961,7 @@
         <v>73.883529967452077</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>81</v>
       </c>
@@ -19983,7 +19987,7 @@
         <v>71.188246673020444</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>82</v>
       </c>
@@ -20009,7 +20013,7 @@
         <v>73.861061983271028</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>83</v>
       </c>
@@ -20035,7 +20039,7 @@
         <v>69.173931927951557</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>84</v>
       </c>
@@ -20061,7 +20065,7 @@
         <v>75.45643850291053</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>85</v>
       </c>
@@ -20100,9 +20104,9 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -20110,7 +20114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -20118,7 +20122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -20126,147 +20130,147 @@
         <v>45405</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>129</v>
       </c>
@@ -20274,62 +20278,62 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>142</v>
       </c>

</xml_diff>